<commit_message>
feat: update excel wording + update helpers values
</commit_message>
<xml_diff>
--- a/formulaire/public/template/template-enfants-v1.xlsx
+++ b/formulaire/public/template/template-enfants-v1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rlega\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F456C363-A745-4AE5-9C8C-204E3A8494B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A57F547A-F88D-4890-B525-80CEFDA7ABD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mode d'emploi" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="83">
   <si>
     <t>Bienvenue sur le template de demande d'autorisations de travail pour les enfants de moins de 16 ans dans le secteur du spectacle.</t>
   </si>
@@ -366,6 +366,18 @@
   </si>
   <si>
     <t>Lieu de travail</t>
+  </si>
+  <si>
+    <t>N° de rue du représentant légal 1</t>
+  </si>
+  <si>
+    <t>Libellé de voie du représentant légal 1</t>
+  </si>
+  <si>
+    <t>Code postal du représentant légal 1</t>
+  </si>
+  <si>
+    <t>Ville du représentant légal 1</t>
   </si>
 </sst>
 </file>
@@ -7159,9 +7171,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Feuil2"/>
-  <dimension ref="A1:AH306"/>
+  <dimension ref="A1:AJ306"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V1" sqref="V1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
@@ -7244,16 +7258,16 @@
         <v>26</v>
       </c>
       <c r="S1" s="9" t="s">
-        <v>27</v>
+        <v>79</v>
       </c>
       <c r="T1" s="9" t="s">
-        <v>28</v>
+        <v>80</v>
       </c>
       <c r="U1" s="9" t="s">
-        <v>29</v>
+        <v>81</v>
       </c>
       <c r="V1" s="9" t="s">
-        <v>30</v>
+        <v>82</v>
       </c>
       <c r="W1" s="9" t="s">
         <v>31</v>
@@ -7295,7 +7309,7 @@
     <row r="2" spans="1:34" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13">
         <f ca="1">TODAY()</f>
-        <v>45042</v>
+        <v>45062</v>
       </c>
       <c r="B2" s="14"/>
       <c r="C2" s="15"/>

</xml_diff>

<commit_message>
feat: update excel wording + update helpers values (#543)
</commit_message>
<xml_diff>
--- a/formulaire/public/template/template-enfants-v1.xlsx
+++ b/formulaire/public/template/template-enfants-v1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rlega\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F456C363-A745-4AE5-9C8C-204E3A8494B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A57F547A-F88D-4890-B525-80CEFDA7ABD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mode d'emploi" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="83">
   <si>
     <t>Bienvenue sur le template de demande d'autorisations de travail pour les enfants de moins de 16 ans dans le secteur du spectacle.</t>
   </si>
@@ -366,6 +366,18 @@
   </si>
   <si>
     <t>Lieu de travail</t>
+  </si>
+  <si>
+    <t>N° de rue du représentant légal 1</t>
+  </si>
+  <si>
+    <t>Libellé de voie du représentant légal 1</t>
+  </si>
+  <si>
+    <t>Code postal du représentant légal 1</t>
+  </si>
+  <si>
+    <t>Ville du représentant légal 1</t>
   </si>
 </sst>
 </file>
@@ -7159,9 +7171,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Feuil2"/>
-  <dimension ref="A1:AH306"/>
+  <dimension ref="A1:AJ306"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V1" sqref="V1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
@@ -7244,16 +7258,16 @@
         <v>26</v>
       </c>
       <c r="S1" s="9" t="s">
-        <v>27</v>
+        <v>79</v>
       </c>
       <c r="T1" s="9" t="s">
-        <v>28</v>
+        <v>80</v>
       </c>
       <c r="U1" s="9" t="s">
-        <v>29</v>
+        <v>81</v>
       </c>
       <c r="V1" s="9" t="s">
-        <v>30</v>
+        <v>82</v>
       </c>
       <c r="W1" s="9" t="s">
         <v>31</v>
@@ -7295,7 +7309,7 @@
     <row r="2" spans="1:34" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13">
         <f ca="1">TODAY()</f>
-        <v>45042</v>
+        <v>45062</v>
       </c>
       <c r="B2" s="14"/>
       <c r="C2" s="15"/>

</xml_diff>